<commit_message>
Completed board and added stencil
</commit_message>
<xml_diff>
--- a/Breakout Board/eeARM BOM.xlsx
+++ b/Breakout Board/eeARM BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>65M2636-H</t>
   </si>
@@ -120,14 +120,98 @@
     <t>PCB</t>
   </si>
   <si>
-    <t>?</t>
+    <t>72M3690</t>
+  </si>
+  <si>
+    <t>B17300 T/R</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SMD 6x3.7 H=2.5</t>
+  </si>
+  <si>
+    <t>72M1139</t>
+  </si>
+  <si>
+    <t>BH341-3A</t>
+  </si>
+  <si>
+    <t>HOLD BAT 4xAA LEAD BK IIII</t>
+  </si>
+  <si>
+    <t>72M3263</t>
+  </si>
+  <si>
+    <t>YY09C02</t>
+  </si>
+  <si>
+    <t>HOUSING SIL 2W 2.54 YY09C02</t>
+  </si>
+  <si>
+    <t>Batteries AA</t>
+  </si>
+  <si>
+    <t>Total per Unit</t>
+  </si>
+  <si>
+    <t>No Units</t>
+  </si>
+  <si>
+    <t>Total cost</t>
+  </si>
+  <si>
+    <t>Per Unit</t>
+  </si>
+  <si>
+    <t>Rubber feet</t>
+  </si>
+  <si>
+    <t>M3 Nut</t>
+  </si>
+  <si>
+    <t>M3 6mm</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Fastener</t>
+  </si>
+  <si>
+    <t>Actionbolt Order</t>
+  </si>
+  <si>
+    <t>Mantech Order</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>M3 8mm</t>
+  </si>
+  <si>
+    <t>M3 10mm</t>
+  </si>
+  <si>
+    <t>M3 12mm</t>
+  </si>
+  <si>
+    <t>M3 20mm</t>
+  </si>
+  <si>
+    <t>TERMINAL YY09/4000 SERIES 2.54</t>
+  </si>
+  <si>
+    <t>YY09CT</t>
+  </si>
+  <si>
+    <t>14M3259</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,16 +243,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF284775"/>
+      <name val="Lucida Sans"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Lucida Sans"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -312,7 +418,100 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -325,7 +524,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -338,14 +537,44 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -353,37 +582,98 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -713,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -725,283 +1015,724 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:15" ht="16" thickBot="1">
+      <c r="A1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="H1" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="L1" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+    </row>
+    <row r="2" spans="1:15" ht="16" thickBot="1">
+      <c r="A2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13">
         <v>11.111111111111111</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="14">
         <f>E2*B2</f>
         <v>11.111111111111111</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
+      <c r="H2" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="45">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="46">
         <v>0.03</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="47">
         <f>E3*B3</f>
         <v>0.12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
+      <c r="H3" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="40">
+        <v>10</v>
+      </c>
+      <c r="J3" s="41">
+        <f>I3*50*1.2</f>
+        <v>600</v>
+      </c>
+      <c r="L3" s="44" t="str">
+        <f>A3</f>
+        <v>RES SMD 0805 2% 10K</v>
+      </c>
+      <c r="M3" s="45" t="str">
+        <f>C3</f>
+        <v>65M2636-H</v>
+      </c>
+      <c r="N3" s="45" t="str">
+        <f>D3</f>
+        <v>MCR10EZHUG103</v>
+      </c>
+      <c r="O3" s="52">
+        <f t="shared" ref="O3:O12" si="0">ROUND(B3*$F$21*1.1, 0)</f>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="45">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="46">
         <v>0.33</v>
       </c>
-      <c r="F4" s="5">
-        <f t="shared" ref="F4:F13" si="0">E4*B4</f>
+      <c r="F4" s="47">
+        <f t="shared" ref="F4:F19" si="1">E4*B4</f>
         <v>0.33</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
+      <c r="H4" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="33">
+        <v>9</v>
+      </c>
+      <c r="J4" s="41">
+        <f t="shared" ref="J4:J9" si="2">I4*50*1.2</f>
+        <v>540</v>
+      </c>
+      <c r="L4" s="44" t="str">
+        <f t="shared" ref="L4:L13" si="3">A4</f>
+        <v>CAP CER SMD 0805 X5R 10uF 10</v>
+      </c>
+      <c r="M4" s="45" t="str">
+        <f t="shared" ref="M4:M13" si="4">C4</f>
+        <v>35M0284</v>
+      </c>
+      <c r="N4" s="45" t="str">
+        <f t="shared" ref="N4:N13" si="5">D4</f>
+        <v>C0805KKX5R6BB106</v>
+      </c>
+      <c r="O4" s="52">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="45">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="46">
         <v>0.3</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="47">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="33">
+        <v>12</v>
+      </c>
+      <c r="J5" s="41">
+        <f t="shared" si="2"/>
+        <v>720</v>
+      </c>
+      <c r="L5" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>CAP CER SMD 0805 NPO 100pF 50</v>
+      </c>
+      <c r="M5" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>35M3582</v>
+      </c>
+      <c r="N5" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>C0805JRNPO9BN101</v>
+      </c>
+      <c r="O5" s="52">
         <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="45">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="45">
         <v>1.29</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="47">
+        <f t="shared" si="1"/>
+        <v>1.29</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="33">
+        <v>3</v>
+      </c>
+      <c r="J6" s="41">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="L6" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>DIODE SKY SOD123 20V 1A MBR120</v>
+      </c>
+      <c r="M6" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>35M4205</v>
+      </c>
+      <c r="N6" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>MBR120LSFT1G</v>
+      </c>
+      <c r="O6" s="52">
         <f t="shared" si="0"/>
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="45">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="45">
         <v>2.0499999999999998</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="47">
+        <f t="shared" si="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="33">
+        <v>7</v>
+      </c>
+      <c r="J7" s="41">
+        <f t="shared" si="2"/>
+        <v>420</v>
+      </c>
+      <c r="L7" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>REG FIX POS SOT223 3V3 1A2</v>
+      </c>
+      <c r="M7" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>82M0939</v>
+      </c>
+      <c r="N7" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>LD1117S33TR</v>
+      </c>
+      <c r="O7" s="52">
         <f t="shared" si="0"/>
-        <v>2.0499999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="45">
         <v>0.5</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="45">
         <v>3.21</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="47">
+        <f t="shared" si="1"/>
+        <v>1.605</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="33">
+        <v>4</v>
+      </c>
+      <c r="J8" s="41">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="L8" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>HEADER SIL STR 40W 2.54 TH=12</v>
+      </c>
+      <c r="M8" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>64M0074</v>
+      </c>
+      <c r="N8" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>PHSS40G1/RH</v>
+      </c>
+      <c r="O8" s="52">
         <f t="shared" si="0"/>
-        <v>1.605</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="16" thickBot="1">
+      <c r="A9" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="45">
         <v>0.5</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="45">
         <v>9.84</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="47">
+        <f t="shared" si="1"/>
+        <v>4.92</v>
+      </c>
+      <c r="H9" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="43">
+        <v>4</v>
+      </c>
+      <c r="J9" s="41">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="L9" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>SOCKET SIL STR HOUSED 2.54 40W</v>
+      </c>
+      <c r="M9" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>14M6379</v>
+      </c>
+      <c r="N9" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>FHSS40G1</v>
+      </c>
+      <c r="O9" s="52">
         <f t="shared" si="0"/>
-        <v>4.92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="45">
+        <v>1</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="45">
+        <v>6.51</v>
+      </c>
+      <c r="F10" s="47">
+        <f t="shared" si="1"/>
+        <v>6.51</v>
+      </c>
+      <c r="L10" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>SWITCH TACTILE SMD 6x3.7 H=2.5</v>
+      </c>
+      <c r="M10" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>72M3690</v>
+      </c>
+      <c r="N10" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>B17300 T/R</v>
+      </c>
+      <c r="O10" s="52">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="45">
+        <v>1</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="45">
+        <v>9</v>
+      </c>
+      <c r="F11" s="47">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="L11" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>HOLD BAT 4xAA LEAD BK IIII</v>
+      </c>
+      <c r="M11" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>72M1139</v>
+      </c>
+      <c r="N11" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>BH341-3A</v>
+      </c>
+      <c r="O11" s="52">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="45">
+        <v>1</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="45">
+        <v>0.67</v>
+      </c>
+      <c r="F12" s="52">
+        <f t="shared" si="1"/>
+        <v>0.67</v>
+      </c>
+      <c r="L12" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>HOUSING SIL 2W 2.54 YY09C02</v>
+      </c>
+      <c r="M12" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>72M3263</v>
+      </c>
+      <c r="N12" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>YY09C02</v>
+      </c>
+      <c r="O12" s="52">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="16" thickBot="1">
+      <c r="A13" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="45">
+        <v>2</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="45">
+        <v>0.43</v>
+      </c>
+      <c r="F13" s="52">
+        <f t="shared" si="1"/>
+        <v>0.86</v>
+      </c>
+      <c r="L13" s="53" t="str">
+        <f t="shared" si="3"/>
+        <v>TERMINAL YY09/4000 SERIES 2.54</v>
+      </c>
+      <c r="M13" s="54" t="str">
+        <f t="shared" si="4"/>
+        <v>14M3259</v>
+      </c>
+      <c r="N13" s="54" t="str">
+        <f t="shared" si="5"/>
+        <v>YY09CT</v>
+      </c>
+      <c r="O13" s="55">
+        <f>ROUND(B13*$F$21*1.2, 0)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B14" s="2">
         <v>4</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
         <v>25</v>
       </c>
-      <c r="F10" s="5">
-        <f t="shared" si="0"/>
+      <c r="F14" s="15">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
+    <row r="15" spans="1:15">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
         <v>50</v>
       </c>
-      <c r="F11" s="5">
-        <f t="shared" si="0"/>
+      <c r="F15" s="15">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4" t="s">
+    <row r="16" spans="1:15">
+      <c r="A16" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B16" s="33">
         <v>1</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3">
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33">
+        <v>40</v>
+      </c>
+      <c r="F16" s="34">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="5">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="16" thickBot="1">
-      <c r="A14" s="14" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3">
+        <v>25</v>
+      </c>
+      <c r="F17" s="15">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" ht="16" thickBot="1">
-      <c r="A15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20">
-        <f>SUM(F2:F14)</f>
-        <v>201.72611111111109</v>
-      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3">
+        <v>75</v>
+      </c>
+      <c r="F18" s="15">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="16" thickBot="1">
+      <c r="A19" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="20">
+        <v>4</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21">
+        <v>5</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="16" thickBot="1">
+      <c r="A20" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="29">
+        <f>SUM(F2:F19)</f>
+        <v>348.76611111111112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="16" thickBot="1">
+      <c r="A21" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="16" thickBot="1">
+      <c r="A22" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="31">
+        <f>F21*F20</f>
+        <v>17438.305555555555</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>